<commit_message>
Now storage works and production values are not huge
</commit_message>
<xml_diff>
--- a/META_final_with_storage.xlsx
+++ b/META_final_with_storage.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5ECD3FE-3B4E-4FAC-8430-BC4149108A01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CC6084-387E-4C4F-B5D9-60652B91BECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3624" yWindow="3324" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4116" yWindow="3540" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -821,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G71" sqref="G71"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -894,7 +894,7 @@
         <v>24</v>
       </c>
       <c r="E4">
-        <v>280.67857754913462</v>
+        <v>135.970057925482</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -939,7 +939,7 @@
         <v>24</v>
       </c>
       <c r="E7">
-        <v>240.87320860346512</v>
+        <v>116.68701050323831</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -984,7 +984,7 @@
         <v>24</v>
       </c>
       <c r="E10">
-        <v>224.54290063383132</v>
+        <v>108.77606503685921</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1029,7 +1029,7 @@
         <v>24</v>
       </c>
       <c r="E13">
-        <v>280.67862579228898</v>
+        <v>135.97008129607386</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1074,7 +1074,7 @@
         <v>24</v>
       </c>
       <c r="E16">
-        <v>255.16238708389929</v>
+        <v>123.60916481461271</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -1119,7 +1119,7 @@
         <v>24</v>
       </c>
       <c r="E19">
-        <v>313.33941133902812</v>
+        <v>151.79205439234426</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1164,7 +1164,7 @@
         <v>24</v>
       </c>
       <c r="E22">
-        <v>318.44265908070599</v>
+        <v>154.26423768863671</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1209,7 +1209,7 @@
         <v>24</v>
       </c>
       <c r="E25">
-        <v>290.8851212756457</v>
+        <v>140.91444788865843</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1254,7 +1254,7 @@
         <v>24</v>
       </c>
       <c r="E28">
-        <v>352.12409417578073</v>
+        <v>170.58064744416549</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1299,7 +1299,7 @@
         <v>24</v>
       </c>
       <c r="E31">
-        <v>377.64033288417096</v>
+        <v>182.94156392562687</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1362,7 +1362,7 @@
         <v>24</v>
       </c>
       <c r="E37">
-        <v>255.87684176773413</v>
+        <v>123.95527047609363</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1407,7 +1407,7 @@
         <v>24</v>
       </c>
       <c r="E40">
-        <v>320.89221799671157</v>
+        <v>155.45088567085691</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1452,7 +1452,7 @@
         <v>24</v>
       </c>
       <c r="E43">
-        <v>380.49815161951017</v>
+        <v>184.32598657155032</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1497,7 +1497,7 @@
         <v>24</v>
       </c>
       <c r="E46">
-        <v>267.92050643809398</v>
+        <v>129.78962305534324</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1542,7 +1542,7 @@
         <v>24</v>
       </c>
       <c r="E49">
-        <v>399.27810330888536</v>
+        <v>193.42362110190592</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -1587,7 +1587,7 @@
         <v>24</v>
       </c>
       <c r="E52">
-        <v>260.26563482557714</v>
+        <v>126.08134811090491</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -1632,7 +1632,7 @@
         <v>24</v>
       </c>
       <c r="E55">
-        <v>274.55472850227551</v>
+        <v>133.00346134052322</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -1677,7 +1677,7 @@
         <v>24</v>
       </c>
       <c r="E58">
-        <v>317.93233430653845</v>
+        <v>154.01701935900746</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -1722,7 +1722,7 @@
         <v>24</v>
       </c>
       <c r="E61">
-        <v>260.67389464491134</v>
+        <v>126.2791227746083</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -1767,7 +1767,7 @@
         <v>24</v>
       </c>
       <c r="E64">
-        <v>485.42092518840991</v>
+        <v>235.15407514331923</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -1812,7 +1812,7 @@
         <v>24</v>
       </c>
       <c r="E67">
-        <v>175.44965735888914</v>
+        <v>84.993661726527705</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -1857,7 +1857,7 @@
         <v>24</v>
       </c>
       <c r="E70">
-        <v>327.11818024155855</v>
+        <v>158.46694929233325</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -1902,7 +1902,7 @@
         <v>24</v>
       </c>
       <c r="E73">
-        <v>481.33832699506729</v>
+        <v>233.17632850628524</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>